<commit_message>
Add new files and update existing files
</commit_message>
<xml_diff>
--- a/data/Source Data.xlsx
+++ b/data/Source Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianiranzetti/Github/Monetary-policy-effect-on-Stock-Prices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianiranzetti/Github/Monetary-policy-effect-on-Stock-Prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B4A92A-141B-6148-B460-839185ED2007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201F7297-E249-F746-BC9D-3A6C5AE1D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="500" windowWidth="14200" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page + Variables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="445">
   <si>
     <t>Date</t>
   </si>
@@ -1365,6 +1365,15 @@
   <si>
     <t>Market Yield on U.S. Treasury Securities at 1-Year Constant Maturity, Quoted on an Investment Basis, Percent, Monthly, Not Seasonally Adjusted</t>
   </si>
+  <si>
+    <t>https://github.com/marekjarocinski</t>
+  </si>
+  <si>
+    <t>surprise in the "policy indicator", ie the 1st principal component of the surprises in interest rate derivatives with maturities from 1 month to 1 year</t>
+  </si>
+  <si>
+    <t>surprise in the S&amp;P500</t>
+  </si>
 </sst>
 </file>
 
@@ -1376,7 +1385,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1439,6 +1448,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1505,7 +1522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1617,6 +1634,7 @@
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1923,10 +1941,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1974,163 +1992,185 @@
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
-        <v>414</v>
+      <c r="A12" s="39" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>415</v>
+        <v>435</v>
       </c>
       <c r="B13" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>417</v>
-      </c>
-    </row>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>436</v>
+      </c>
+      <c r="B14" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B16" t="s">
-        <v>418</v>
+      <c r="A16" s="33" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>415</v>
       </c>
       <c r="B17" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>420</v>
-      </c>
-    </row>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>440</v>
-      </c>
-      <c r="B19" t="s">
-        <v>441</v>
+      <c r="A19" s="33" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>6</v>
+      <c r="A20" t="s">
+        <v>404</v>
       </c>
       <c r="B20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>420</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
-        <v>422</v>
+      <c r="A23" t="s">
+        <v>440</v>
+      </c>
+      <c r="B23" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>438</v>
       </c>
       <c r="B25" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
-        <v>425</v>
-      </c>
-    </row>
+        <v>439</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>426</v>
+      <c r="A27" s="33" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>433</v>
       </c>
     </row>
@@ -2146,8 +2186,8 @@
   </sheetPr>
   <dimension ref="A1:W387"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>